<commit_message>
Update KOTAK_DB.ipynb and related data outputs
Added new library imports and updated code cells in KOTAK_DB.ipynb, including execution counts and output logs for data processing and database operations. Updated several output Excel files and Power BI dashboard, and removed the obsolete atom_report_clean.xlsx file.
</commit_message>
<xml_diff>
--- a/output_data/atom_report_cleaned.xlsx
+++ b/output_data/atom_report_cleaned.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL37"/>
+  <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1387,28 +1387,32 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>17259</v>
+        <v>17260</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SIDDI SHANMUKHA SESA SAI DHANUSH</t>
+          <t>SIDDI SHANMUKHA SAI MANI DEEPANSH</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>6305761566</v>
       </c>
       <c r="D7" t="n">
-        <v>10750</v>
+        <v>8850</v>
       </c>
       <c r="E7" t="n">
-        <v>11250</v>
+        <v>8850</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>31-Oct-2025 19:33:22</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+          <t>31-Oct-2025 19:34:18</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>01-Nov-2025 00:00:00</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
@@ -1421,16 +1425,16 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>VlllX</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>eleven thousand two hundred fifty</t>
+          <t>eight thousand eight hundred fifty</t>
         </is>
       </c>
       <c r="L7" t="n">
-        <v>899053000000003</v>
+        <v>100000036600</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -1444,13 +1448,13 @@
         <v>1234</v>
       </c>
       <c r="P7" t="n">
-        <v>11000313779340</v>
+        <v>11000313779393</v>
       </c>
       <c r="Q7" t="n">
-        <v>1761918525</v>
+        <v>1761919447</v>
       </c>
       <c r="R7" t="n">
-        <v>712356161457</v>
+        <v>515333448324</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1469,7 +1473,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>RNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
@@ -1507,7 +1511,11 @@
       <c r="AE7" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr">
         <is>
@@ -1515,16 +1523,16 @@
         </is>
       </c>
       <c r="AI7" t="n">
-        <v>19971</v>
+        <v>19972</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>263200,264703</t>
+          <t>262662,264219</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>2037,2044</t>
+          <t>2037,2042</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
@@ -1535,30 +1543,30 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>17259</v>
+        <v>15863</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SIDDI SHANMUKHA SESA SAI DHANUSH</t>
+          <t>BOMMIDI BALA SURYA BHUVAN</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6305761566</v>
+        <v>6300875193</v>
       </c>
       <c r="D8" t="n">
-        <v>500</v>
+        <v>8050</v>
       </c>
       <c r="E8" t="n">
-        <v>11250</v>
+        <v>8050</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>31-Oct-2025 19:33:22</t>
+          <t>01-Nov-2025 08:31:08</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>01-Nov-2025 00:00:00</t>
+          <t>03-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1578,11 +1586,11 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>eleven thousand two hundred fifty</t>
+          <t>eight thousand fifty</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>899053000000002</v>
+        <v>100000036600</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -1596,13 +1604,13 @@
         <v>1234</v>
       </c>
       <c r="P8" t="n">
-        <v>11000313779340</v>
+        <v>11000313842066</v>
       </c>
       <c r="Q8" t="n">
-        <v>1761918525</v>
+        <v>1761966017</v>
       </c>
       <c r="R8" t="n">
-        <v>712356161457</v>
+        <v>530592204041</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1659,7 +1667,11 @@
       <c r="AE8" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr">
         <is>
@@ -1667,50 +1679,46 @@
         </is>
       </c>
       <c r="AI8" t="n">
-        <v>19971</v>
+        <v>18543</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>263200,264703</t>
+          <t>261028</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>2037,2044</t>
-        </is>
-      </c>
-      <c r="AL8" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2032</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17260</v>
+        <v>16641</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SIDDI SHANMUKHA SAI MANI DEEPANSH</t>
+          <t>KETHA DHANVI REDDY</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6305761566</v>
+        <v>7673910081</v>
       </c>
       <c r="D9" t="n">
-        <v>8850</v>
+        <v>8250</v>
       </c>
       <c r="E9" t="n">
-        <v>8850</v>
+        <v>8250</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>31-Oct-2025 19:34:18</t>
+          <t>01-Nov-2025 18:41:39</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>01-Nov-2025 00:00:00</t>
+          <t>03-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1730,7 +1738,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>eight thousand eight hundred fifty</t>
+          <t>eight thousand two hundred fifty</t>
         </is>
       </c>
       <c r="L9" t="n">
@@ -1748,13 +1756,13 @@
         <v>1234</v>
       </c>
       <c r="P9" t="n">
-        <v>11000313779393</v>
+        <v>11000313935521</v>
       </c>
       <c r="Q9" t="n">
-        <v>1761919447</v>
+        <v>1762002237</v>
       </c>
       <c r="R9" t="n">
-        <v>515333448324</v>
+        <v>530595643689</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -1823,45 +1831,41 @@
         </is>
       </c>
       <c r="AI9" t="n">
-        <v>19972</v>
+        <v>18181</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>262662,264219</t>
+          <t>262111,263519</t>
         </is>
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>2037,2042</t>
-        </is>
-      </c>
-      <c r="AL9" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2037,2040</t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15863</v>
+        <v>16262</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BOMMIDI BALA SURYA BHUVAN</t>
+          <t>KETHA VIDHAT REDDY</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6300875193</v>
+        <v>7673910081</v>
       </c>
       <c r="D10" t="n">
-        <v>8050</v>
+        <v>8550</v>
       </c>
       <c r="E10" t="n">
-        <v>8050</v>
+        <v>8550</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>01-Nov-2025 08:31:08</t>
+          <t>01-Nov-2025 18:44:10</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1886,7 +1890,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>eight thousand fifty</t>
+          <t>eight thousand five hundred fifty</t>
         </is>
       </c>
       <c r="L10" t="n">
@@ -1904,13 +1908,13 @@
         <v>1234</v>
       </c>
       <c r="P10" t="n">
-        <v>11000313842066</v>
+        <v>11000313935621</v>
       </c>
       <c r="Q10" t="n">
-        <v>1761966017</v>
+        <v>1762002807</v>
       </c>
       <c r="R10" t="n">
-        <v>530592204041</v>
+        <v>530595660270</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1979,31 +1983,31 @@
         </is>
       </c>
       <c r="AI10" t="n">
-        <v>18543</v>
+        <v>18444</v>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>261028</t>
+          <t>262243,263840</t>
         </is>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>2032</t>
+          <t>2037,2041</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16641</v>
+        <v>16981</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KETHA DHANVI REDDY</t>
+          <t>NISCHAL BENEDICT THOTA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7673910081</v>
+        <v>8919560551</v>
       </c>
       <c r="D11" t="n">
         <v>8250</v>
@@ -2013,7 +2017,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>01-Nov-2025 18:41:39</t>
+          <t>01-Nov-2025 19:07:23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -2056,13 +2060,13 @@
         <v>1234</v>
       </c>
       <c r="P11" t="n">
-        <v>11000313935521</v>
+        <v>11000313938477</v>
       </c>
       <c r="Q11" t="n">
-        <v>1762002237</v>
+        <v>1762004142</v>
       </c>
       <c r="R11" t="n">
-        <v>530595643689</v>
+        <v>530595804803</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -2131,11 +2135,11 @@
         </is>
       </c>
       <c r="AI11" t="n">
-        <v>18181</v>
+        <v>18142</v>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>262111,263519</t>
+          <t>262680,263610</t>
         </is>
       </c>
       <c r="AK11" t="inlineStr">
@@ -2147,25 +2151,25 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16262</v>
+        <v>17283</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KETHA VIDHAT REDDY</t>
+          <t>DODDI KUSHAL GOWTHAM</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7673910081</v>
+        <v>9014001763</v>
       </c>
       <c r="D12" t="n">
-        <v>8550</v>
+        <v>6750</v>
       </c>
       <c r="E12" t="n">
-        <v>8550</v>
+        <v>6750</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>01-Nov-2025 18:44:10</t>
+          <t>01-Nov-2025 19:42:41</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2185,12 +2189,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>eight thousand five hundred fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L12" t="n">
@@ -2208,13 +2212,13 @@
         <v>1234</v>
       </c>
       <c r="P12" t="n">
-        <v>11000313935621</v>
+        <v>11000313943507</v>
       </c>
       <c r="Q12" t="n">
-        <v>1762002807</v>
+        <v>1762006130</v>
       </c>
       <c r="R12" t="n">
-        <v>530595660270</v>
+        <v>113502707585</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -2273,7 +2277,7 @@
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -2283,41 +2287,45 @@
         </is>
       </c>
       <c r="AI12" t="n">
-        <v>18444</v>
+        <v>19994</v>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
-          <t>262243,263840</t>
+          <t>263376</t>
         </is>
       </c>
       <c r="AK12" t="inlineStr">
         <is>
-          <t>2037,2041</t>
-        </is>
-      </c>
-      <c r="AL12" t="inlineStr"/>
+          <t>2039</t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16981</v>
+        <v>15544</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NISCHAL BENEDICT THOTA</t>
+          <t>BANNARAVURI JAI AADHITHYA SHIVA SATWIK</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8919560551</v>
+        <v>9866667129</v>
       </c>
       <c r="D13" t="n">
-        <v>8250</v>
+        <v>8850</v>
       </c>
       <c r="E13" t="n">
-        <v>8250</v>
+        <v>8850</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>01-Nov-2025 19:07:23</t>
+          <t>02-Nov-2025 06:36:19</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -2342,7 +2350,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>eight thousand two hundred fifty</t>
+          <t>eight thousand eight hundred fifty</t>
         </is>
       </c>
       <c r="L13" t="n">
@@ -2360,13 +2368,13 @@
         <v>1234</v>
       </c>
       <c r="P13" t="n">
-        <v>11000313938477</v>
+        <v>11000313995786</v>
       </c>
       <c r="Q13" t="n">
-        <v>1762004142</v>
+        <v>1762045566</v>
       </c>
       <c r="R13" t="n">
-        <v>530595804803</v>
+        <v>785956568564</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
@@ -2435,41 +2443,45 @@
         </is>
       </c>
       <c r="AI13" t="n">
-        <v>18142</v>
+        <v>18968</v>
       </c>
       <c r="AJ13" t="inlineStr">
         <is>
-          <t>262680,263610</t>
+          <t>262798,264301</t>
         </is>
       </c>
       <c r="AK13" t="inlineStr">
         <is>
-          <t>2037,2040</t>
-        </is>
-      </c>
-      <c r="AL13" t="inlineStr"/>
+          <t>2037,2042</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>17283</v>
+        <v>16710</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DODDI KUSHAL GOWTHAM</t>
+          <t>BANNARAVURI HIMAKSHARA</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9014001763</v>
+        <v>9866667129</v>
       </c>
       <c r="D14" t="n">
-        <v>6750</v>
+        <v>8250</v>
       </c>
       <c r="E14" t="n">
-        <v>6750</v>
+        <v>8250</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>01-Nov-2025 19:42:41</t>
+          <t>02-Nov-2025 06:29:05</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -2489,12 +2501,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>PREKGUKG</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>six thousand seven hundred fifty</t>
+          <t>eight thousand two hundred fifty</t>
         </is>
       </c>
       <c r="L14" t="n">
@@ -2512,13 +2524,13 @@
         <v>1234</v>
       </c>
       <c r="P14" t="n">
-        <v>11000313943507</v>
+        <v>11000313996665</v>
       </c>
       <c r="Q14" t="n">
-        <v>1762006130</v>
+        <v>1762045034</v>
       </c>
       <c r="R14" t="n">
-        <v>113502707585</v>
+        <v>918689336704</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -2577,7 +2589,7 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -2587,16 +2599,16 @@
         </is>
       </c>
       <c r="AI14" t="n">
-        <v>19994</v>
+        <v>18184</v>
       </c>
       <c r="AJ14" t="inlineStr">
         <is>
-          <t>263376</t>
+          <t>262011,263504</t>
         </is>
       </c>
       <c r="AK14" t="inlineStr">
         <is>
-          <t>2039</t>
+          <t>2037,2040</t>
         </is>
       </c>
       <c r="AL14" t="inlineStr">
@@ -2607,25 +2619,25 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16710</v>
+        <v>17175</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BANNARAVURI HIMAKSHARA</t>
+          <t>DWARAMPUDI MOKSHITA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>9866667129</v>
+        <v>9505754523</v>
       </c>
       <c r="D15" t="n">
-        <v>8250</v>
+        <v>6750</v>
       </c>
       <c r="E15" t="n">
-        <v>8250</v>
+        <v>6750</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>02-Nov-2025 06:29:05</t>
+          <t>02-Nov-2025 13:55:05</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -2645,12 +2657,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>eight thousand two hundred fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L15" t="n">
@@ -2668,13 +2680,13 @@
         <v>1234</v>
       </c>
       <c r="P15" t="n">
-        <v>11000313996665</v>
+        <v>11000314043670</v>
       </c>
       <c r="Q15" t="n">
-        <v>1762045034</v>
+        <v>1762071875</v>
       </c>
       <c r="R15" t="n">
-        <v>918689336704</v>
+        <v>530699877652</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
@@ -2733,7 +2745,7 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -2743,45 +2755,41 @@
         </is>
       </c>
       <c r="AI15" t="n">
-        <v>18184</v>
+        <v>19890</v>
       </c>
       <c r="AJ15" t="inlineStr">
         <is>
-          <t>262011,263504</t>
+          <t>264989</t>
         </is>
       </c>
       <c r="AK15" t="inlineStr">
         <is>
-          <t>2037,2040</t>
-        </is>
-      </c>
-      <c r="AL15" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2047</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15544</v>
+        <v>16686</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BANNARAVURI JAI AADHITHYA SHIVA SATWIK</t>
+          <t>DWARAMPUDI BHUVAN REDDY</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>9866667129</v>
+        <v>9505754523</v>
       </c>
       <c r="D16" t="n">
-        <v>8850</v>
+        <v>8050</v>
       </c>
       <c r="E16" t="n">
-        <v>8850</v>
+        <v>8050</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>02-Nov-2025 06:36:19</t>
+          <t>02-Nov-2025 13:51:20</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -2806,7 +2814,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>eight thousand eight hundred fifty</t>
+          <t>eight thousand fifty</t>
         </is>
       </c>
       <c r="L16" t="n">
@@ -2824,13 +2832,13 @@
         <v>1234</v>
       </c>
       <c r="P16" t="n">
-        <v>11000313995786</v>
+        <v>11000314044028</v>
       </c>
       <c r="Q16" t="n">
-        <v>1762045566</v>
+        <v>1762071557</v>
       </c>
       <c r="R16" t="n">
-        <v>785956568564</v>
+        <v>530699856490</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -2899,50 +2907,46 @@
         </is>
       </c>
       <c r="AI16" t="n">
-        <v>18968</v>
+        <v>18393</v>
       </c>
       <c r="AJ16" t="inlineStr">
         <is>
-          <t>262798,264301</t>
+          <t>265461</t>
         </is>
       </c>
       <c r="AK16" t="inlineStr">
         <is>
-          <t>2037,2042</t>
-        </is>
-      </c>
-      <c r="AL16" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2049</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16686</v>
+        <v>17105</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>DWARAMPUDI BHUVAN REDDY</t>
+          <t>AADHVIK DADIRAO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9505754523</v>
+        <v>7075570737</v>
       </c>
       <c r="D17" t="n">
-        <v>8050</v>
+        <v>6750</v>
       </c>
       <c r="E17" t="n">
-        <v>8050</v>
+        <v>6750</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>02-Nov-2025 13:51:20</t>
+          <t>03-Nov-2025 09:40:54</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>03-Nov-2025 00:00:00</t>
+          <t>04-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -2957,12 +2961,12 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>eight thousand fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L17" t="n">
@@ -2980,13 +2984,13 @@
         <v>1234</v>
       </c>
       <c r="P17" t="n">
-        <v>11000314044028</v>
+        <v>11000314169121</v>
       </c>
       <c r="Q17" t="n">
-        <v>1762071557</v>
+        <v>1762143020</v>
       </c>
       <c r="R17" t="n">
-        <v>530699856490</v>
+        <v>195817510674</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -3045,7 +3049,7 @@
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -3055,46 +3059,50 @@
         </is>
       </c>
       <c r="AI17" t="n">
-        <v>18393</v>
+        <v>18096</v>
       </c>
       <c r="AJ17" t="inlineStr">
         <is>
-          <t>265461</t>
+          <t>265123</t>
         </is>
       </c>
       <c r="AK17" t="inlineStr">
         <is>
-          <t>2049</t>
-        </is>
-      </c>
-      <c r="AL17" t="inlineStr"/>
+          <t>2047</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17175</v>
+        <v>15539</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>DWARAMPUDI MOKSHITA</t>
+          <t>MUSKHAN KARRI</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9505754523</v>
+        <v>8019731551</v>
       </c>
       <c r="D18" t="n">
-        <v>6750</v>
+        <v>8350</v>
       </c>
       <c r="E18" t="n">
-        <v>6750</v>
+        <v>8350</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>02-Nov-2025 13:55:05</t>
+          <t>03-Nov-2025 10:43:59</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>03-Nov-2025 00:00:00</t>
+          <t>04-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -3109,12 +3117,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>PREKGUKG</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>six thousand seven hundred fifty</t>
+          <t>eight thousand three hundred fifty</t>
         </is>
       </c>
       <c r="L18" t="n">
@@ -3132,13 +3140,13 @@
         <v>1234</v>
       </c>
       <c r="P18" t="n">
-        <v>11000314043670</v>
+        <v>11000314184250</v>
       </c>
       <c r="Q18" t="n">
-        <v>1762071875</v>
+        <v>1762146594</v>
       </c>
       <c r="R18" t="n">
-        <v>530699877652</v>
+        <v>14573152974</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -3197,7 +3205,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -3207,41 +3215,45 @@
         </is>
       </c>
       <c r="AI18" t="n">
-        <v>19890</v>
+        <v>18875</v>
       </c>
       <c r="AJ18" t="inlineStr">
         <is>
-          <t>264989</t>
+          <t>265913</t>
         </is>
       </c>
       <c r="AK18" t="inlineStr">
         <is>
-          <t>2047</t>
-        </is>
-      </c>
-      <c r="AL18" t="inlineStr"/>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17105</v>
+        <v>17264</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AADHVIK DADIRAO</t>
+          <t>SILUGURI CHIYAN ESHAN VARMA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>7075570737</v>
+        <v>8639375454</v>
       </c>
       <c r="D19" t="n">
-        <v>6750</v>
+        <v>7750</v>
       </c>
       <c r="E19" t="n">
-        <v>6750</v>
+        <v>7750</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>03-Nov-2025 09:40:54</t>
+          <t>03-Nov-2025 11:19:22</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -3261,12 +3273,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>PREKGUKG</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>six thousand seven hundred fifty</t>
+          <t>seven thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L19" t="n">
@@ -3284,13 +3296,13 @@
         <v>1234</v>
       </c>
       <c r="P19" t="n">
-        <v>11000314169121</v>
+        <v>11000314192800</v>
       </c>
       <c r="Q19" t="n">
-        <v>1762143020</v>
+        <v>1762148759</v>
       </c>
       <c r="R19" t="n">
-        <v>195817510674</v>
+        <v>530704742117</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -3349,7 +3361,7 @@
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -3359,45 +3371,41 @@
         </is>
       </c>
       <c r="AI19" t="n">
-        <v>18096</v>
+        <v>19975</v>
       </c>
       <c r="AJ19" t="inlineStr">
         <is>
-          <t>265123</t>
+          <t>260649</t>
         </is>
       </c>
       <c r="AK19" t="inlineStr">
         <is>
-          <t>2047</t>
-        </is>
-      </c>
-      <c r="AL19" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2031</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>15539</v>
+        <v>17264</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MUSKHAN KARRI</t>
+          <t>SILUGURI CHIYAN ESHAN VARMA</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8019731551</v>
+        <v>8639375454</v>
       </c>
       <c r="D20" t="n">
-        <v>8350</v>
+        <v>500</v>
       </c>
       <c r="E20" t="n">
-        <v>8350</v>
+        <v>500</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>03-Nov-2025 10:43:59</t>
+          <t>03-Nov-2025 11:22:01</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -3422,7 +3430,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>eight thousand three hundred fifty</t>
+          <t>five hundred</t>
         </is>
       </c>
       <c r="L20" t="n">
@@ -3440,13 +3448,13 @@
         <v>1234</v>
       </c>
       <c r="P20" t="n">
-        <v>11000314184250</v>
+        <v>11000314194327</v>
       </c>
       <c r="Q20" t="n">
-        <v>1762146594</v>
+        <v>1762149006</v>
       </c>
       <c r="R20" t="n">
-        <v>14573152974</v>
+        <v>530704756640</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -3515,50 +3523,46 @@
         </is>
       </c>
       <c r="AI20" t="n">
-        <v>18875</v>
+        <v>19975</v>
       </c>
       <c r="AJ20" t="inlineStr">
         <is>
-          <t>265913</t>
+          <t>262720</t>
         </is>
       </c>
       <c r="AK20" t="inlineStr">
         <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="AL20" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
+          <t>2037</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>17264</v>
+        <v>17210</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SILUGURI CHIYAN ESHAN VARMA</t>
+          <t>KITLANGI DAKSHITH DURGA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8639375454</v>
+        <v>8985833952</v>
       </c>
       <c r="D21" t="n">
-        <v>7750</v>
+        <v>6750</v>
       </c>
       <c r="E21" t="n">
-        <v>7750</v>
+        <v>6750</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>03-Nov-2025 11:19:22</t>
+          <t>04-Nov-2025 05:47:38</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>04-Nov-2025 00:00:00</t>
+          <t>06-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -3573,12 +3577,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>seven thousand seven hundred fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L21" t="n">
@@ -3596,13 +3600,13 @@
         <v>1234</v>
       </c>
       <c r="P21" t="n">
-        <v>11000314192800</v>
+        <v>11000314371032</v>
       </c>
       <c r="Q21" t="n">
-        <v>1762148759</v>
+        <v>1762215410</v>
       </c>
       <c r="R21" t="n">
-        <v>530704742117</v>
+        <v>530809027996</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -3661,7 +3665,7 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -3671,46 +3675,46 @@
         </is>
       </c>
       <c r="AI21" t="n">
-        <v>19975</v>
+        <v>19924</v>
       </c>
       <c r="AJ21" t="inlineStr">
         <is>
-          <t>260649</t>
+          <t>265130</t>
         </is>
       </c>
       <c r="AK21" t="inlineStr">
         <is>
-          <t>2031</t>
+          <t>2047</t>
         </is>
       </c>
       <c r="AL21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>17264</v>
+        <v>14546</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SILUGURI CHIYAN ESHAN VARMA</t>
+          <t>KONDALA JOSHNA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>8639375454</v>
+        <v>8143411492</v>
       </c>
       <c r="D22" t="n">
-        <v>500</v>
+        <v>11850</v>
       </c>
       <c r="E22" t="n">
-        <v>500</v>
+        <v>11850</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>03-Nov-2025 11:22:01</t>
+          <t>04-Nov-2025 10:01:06</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>04-Nov-2025 00:00:00</t>
+          <t>06-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -3725,12 +3729,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>Multi</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>five hundred</t>
+          <t>eleven thousand eight hundred fifty</t>
         </is>
       </c>
       <c r="L22" t="n">
@@ -3748,13 +3752,13 @@
         <v>1234</v>
       </c>
       <c r="P22" t="n">
-        <v>11000314194327</v>
+        <v>11000314404943</v>
       </c>
       <c r="Q22" t="n">
-        <v>1762149006</v>
+        <v>1762230465</v>
       </c>
       <c r="R22" t="n">
-        <v>530704756640</v>
+        <v>530810055673</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -3773,12 +3777,12 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>RNS</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>SIBL0000899</t>
+          <t>IFSC0000000</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
@@ -3811,11 +3815,7 @@
       <c r="AE22" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF22" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
-        </is>
-      </c>
+      <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr">
         <is>
@@ -3823,41 +3823,41 @@
         </is>
       </c>
       <c r="AI22" t="n">
-        <v>19975</v>
+        <v>19383</v>
       </c>
       <c r="AJ22" t="inlineStr">
         <is>
-          <t>262720</t>
+          <t>263244,264747</t>
         </is>
       </c>
       <c r="AK22" t="inlineStr">
         <is>
-          <t>2037</t>
+          <t>2037,2045</t>
         </is>
       </c>
       <c r="AL22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>17210</v>
+        <v>16868</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KITLANGI DAKSHITH DURGA</t>
+          <t>MULAGAPAKA SALOMI</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8985833952</v>
+        <v>9059539555</v>
       </c>
       <c r="D23" t="n">
-        <v>6750</v>
+        <v>8550</v>
       </c>
       <c r="E23" t="n">
-        <v>6750</v>
+        <v>8550</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>04-Nov-2025 05:47:38</t>
+          <t>04-Nov-2025 12:11:55</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>PREKGUKG</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>six thousand seven hundred fifty</t>
+          <t>eight thousand five hundred fifty</t>
         </is>
       </c>
       <c r="L23" t="n">
@@ -3900,13 +3900,13 @@
         <v>1234</v>
       </c>
       <c r="P23" t="n">
-        <v>11000314371032</v>
+        <v>11000314457730</v>
       </c>
       <c r="Q23" t="n">
-        <v>1762215410</v>
+        <v>1762238461</v>
       </c>
       <c r="R23" t="n">
-        <v>530809027996</v>
+        <v>530810708858</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
       <c r="AG23" t="inlineStr"/>
@@ -3975,41 +3975,41 @@
         </is>
       </c>
       <c r="AI23" t="n">
-        <v>19924</v>
+        <v>18488</v>
       </c>
       <c r="AJ23" t="inlineStr">
         <is>
-          <t>265130</t>
+          <t>262203,263832</t>
         </is>
       </c>
       <c r="AK23" t="inlineStr">
         <is>
-          <t>2047</t>
+          <t>2037,2041</t>
         </is>
       </c>
       <c r="AL23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>14546</v>
+        <v>16895</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KONDALA JOSHNA</t>
+          <t>MULAGAPAKA SAMEER VICTOR</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>8143411492</v>
+        <v>9059539555</v>
       </c>
       <c r="D24" t="n">
-        <v>11850</v>
+        <v>9150</v>
       </c>
       <c r="E24" t="n">
-        <v>11850</v>
+        <v>9150</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>04-Nov-2025 10:01:06</t>
+          <t>04-Nov-2025 12:09:35</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>eleven thousand eight hundred fifty</t>
+          <t>nine thousand one hundred fifty</t>
         </is>
       </c>
       <c r="L24" t="n">
@@ -4052,13 +4052,13 @@
         <v>1234</v>
       </c>
       <c r="P24" t="n">
-        <v>11000314404943</v>
+        <v>11000314458205</v>
       </c>
       <c r="Q24" t="n">
-        <v>1762230465</v>
+        <v>1762238268</v>
       </c>
       <c r="R24" t="n">
-        <v>530810055673</v>
+        <v>530810696020</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -4123,44 +4123,48 @@
         </is>
       </c>
       <c r="AI24" t="n">
-        <v>19383</v>
+        <v>19141</v>
       </c>
       <c r="AJ24" t="inlineStr">
         <is>
-          <t>263244,264747</t>
+          <t>263014,264517</t>
         </is>
       </c>
       <c r="AK24" t="inlineStr">
         <is>
-          <t>2037,2045</t>
+          <t>2037,2043</t>
         </is>
       </c>
       <c r="AL24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>14546</v>
+        <v>17264</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>KONDALA JOSHNA</t>
+          <t>SILUGURI CHIYAN ESHAN VARMA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8143411492</v>
+        <v>8639375454</v>
       </c>
       <c r="D25" t="n">
-        <v>11350</v>
+        <v>7750</v>
       </c>
       <c r="E25" t="n">
-        <v>11850</v>
+        <v>7750</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>04-Nov-2025 10:01:06</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
+          <t>04-Nov-2025 14:59:32</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>06-Nov-2025 00:00:00</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
@@ -4173,16 +4177,16 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>VlllX</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>eleven thousand eight hundred fifty</t>
+          <t>seven thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>899053000000003</v>
+        <v>100000036600</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
@@ -4196,13 +4200,13 @@
         <v>1234</v>
       </c>
       <c r="P25" t="n">
-        <v>11000314404943</v>
+        <v>11000314506510</v>
       </c>
       <c r="Q25" t="n">
-        <v>1762230465</v>
+        <v>1762248487</v>
       </c>
       <c r="R25" t="n">
-        <v>530810055673</v>
+        <v>530811667162</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -4221,7 +4225,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>RNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
@@ -4259,7 +4263,11 @@
       <c r="AE25" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="inlineStr">
         <is>
@@ -4267,41 +4275,41 @@
         </is>
       </c>
       <c r="AI25" t="n">
-        <v>19383</v>
+        <v>19975</v>
       </c>
       <c r="AJ25" t="inlineStr">
         <is>
-          <t>263244,264747</t>
+          <t>263624</t>
         </is>
       </c>
       <c r="AK25" t="inlineStr">
         <is>
-          <t>2037,2045</t>
+          <t>2040</t>
         </is>
       </c>
       <c r="AL25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>14546</v>
+        <v>17188</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>KONDALA JOSHNA</t>
+          <t>REYANA SRIJITH</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>8143411492</v>
+        <v>9985925345</v>
       </c>
       <c r="D26" t="n">
-        <v>500</v>
+        <v>8250</v>
       </c>
       <c r="E26" t="n">
-        <v>11850</v>
+        <v>8250</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>04-Nov-2025 10:01:06</t>
+          <t>04-Nov-2025 23:11:27</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -4326,11 +4334,11 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>eleven thousand eight hundred fifty</t>
+          <t>eight thousand two hundred fifty</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>899053000000002</v>
+        <v>100000036600</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
@@ -4344,13 +4352,13 @@
         <v>1234</v>
       </c>
       <c r="P26" t="n">
-        <v>11000314404943</v>
+        <v>11000314605606</v>
       </c>
       <c r="Q26" t="n">
-        <v>1762230465</v>
+        <v>1762278029</v>
       </c>
       <c r="R26" t="n">
-        <v>530810055673</v>
+        <v>530814184976</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
@@ -4407,7 +4415,11 @@
       <c r="AE26" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="inlineStr">
         <is>
@@ -4415,41 +4427,41 @@
         </is>
       </c>
       <c r="AI26" t="n">
-        <v>19383</v>
+        <v>19902</v>
       </c>
       <c r="AJ26" t="inlineStr">
         <is>
-          <t>263244,264747</t>
+          <t>262289,263690</t>
         </is>
       </c>
       <c r="AK26" t="inlineStr">
         <is>
-          <t>2037,2045</t>
+          <t>2037,2040</t>
         </is>
       </c>
       <c r="AL26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>16895</v>
+        <v>16885</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MULAGAPAKA SAMEER VICTOR</t>
+          <t>JOITA CHETTI</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>9059539555</v>
+        <v>8106613759</v>
       </c>
       <c r="D27" t="n">
-        <v>9150</v>
+        <v>16000</v>
       </c>
       <c r="E27" t="n">
-        <v>9150</v>
+        <v>16000</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>04-Nov-2025 12:09:35</t>
+          <t>05-Nov-2025 07:54:02</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -4469,12 +4481,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Multi</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>nine thousand one hundred fifty</t>
+          <t xml:space="preserve">sixteen thousand </t>
         </is>
       </c>
       <c r="L27" t="n">
@@ -4492,13 +4504,13 @@
         <v>1234</v>
       </c>
       <c r="P27" t="n">
-        <v>11000314458205</v>
+        <v>11000314620667</v>
       </c>
       <c r="Q27" t="n">
-        <v>1762238268</v>
+        <v>1762309313</v>
       </c>
       <c r="R27" t="n">
-        <v>530810696020</v>
+        <v>530915626358</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
@@ -4517,12 +4529,12 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>RNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>IFSC0000000</t>
+          <t>SIBL0000899</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
@@ -4555,7 +4567,11 @@
       <c r="AE27" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="inlineStr">
         <is>
@@ -4563,44 +4579,48 @@
         </is>
       </c>
       <c r="AI27" t="n">
-        <v>19141</v>
+        <v>18185</v>
       </c>
       <c r="AJ27" t="inlineStr">
         <is>
-          <t>263014,264517</t>
+          <t>262047,263508,265158</t>
         </is>
       </c>
       <c r="AK27" t="inlineStr">
         <is>
-          <t>2037,2043</t>
+          <t>2037,2040,2048</t>
         </is>
       </c>
       <c r="AL27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>16895</v>
+        <v>16974</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MULAGAPAKA SAMEER VICTOR</t>
+          <t>KADAJARI ESHAN ESWAR</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9059539555</v>
+        <v>9885130099</v>
       </c>
       <c r="D28" t="n">
-        <v>8650</v>
+        <v>8250</v>
       </c>
       <c r="E28" t="n">
-        <v>9150</v>
+        <v>8250</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>04-Nov-2025 12:09:35</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
+          <t>06-Nov-2025 09:44:46</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>07-Nov-2025 00:00:00</t>
+        </is>
+      </c>
       <c r="H28" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
@@ -4613,16 +4633,16 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Vll</t>
+          <t>lVl</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>nine thousand one hundred fifty</t>
+          <t>eight thousand two hundred fifty</t>
         </is>
       </c>
       <c r="L28" t="n">
-        <v>899053000000004</v>
+        <v>100000036600</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
@@ -4636,13 +4656,13 @@
         <v>1234</v>
       </c>
       <c r="P28" t="n">
-        <v>11000314458205</v>
+        <v>11000314846264</v>
       </c>
       <c r="Q28" t="n">
-        <v>1762238268</v>
+        <v>1762401796</v>
       </c>
       <c r="R28" t="n">
-        <v>530810696020</v>
+        <v>531022524983</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
@@ -4661,7 +4681,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>RNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
@@ -4699,7 +4719,11 @@
       <c r="AE28" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="inlineStr">
         <is>
@@ -4707,46 +4731,46 @@
         </is>
       </c>
       <c r="AI28" t="n">
-        <v>19141</v>
+        <v>18273</v>
       </c>
       <c r="AJ28" t="inlineStr">
         <is>
-          <t>263014,264517</t>
+          <t>262526,263740</t>
         </is>
       </c>
       <c r="AK28" t="inlineStr">
         <is>
-          <t>2037,2043</t>
+          <t>2037,2040</t>
         </is>
       </c>
       <c r="AL28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>16895</v>
+        <v>17229</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MULAGAPAKA SAMEER VICTOR</t>
+          <t>GOLAGANI SOHITHA SAI SANJANA</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>9059539555</v>
+        <v>9985965602</v>
       </c>
       <c r="D29" t="n">
-        <v>500</v>
+        <v>8350</v>
       </c>
       <c r="E29" t="n">
-        <v>9150</v>
+        <v>8350</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>04-Nov-2025 12:09:35</t>
+          <t>06-Nov-2025 11:59:04</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>06-Nov-2025 00:00:00</t>
+          <t>07-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -4766,11 +4790,11 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>nine thousand one hundred fifty</t>
+          <t>eight thousand three hundred fifty</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>899053000000002</v>
+        <v>100000036600</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
@@ -4784,13 +4808,13 @@
         <v>1234</v>
       </c>
       <c r="P29" t="n">
-        <v>11000314458205</v>
+        <v>11000314879817</v>
       </c>
       <c r="Q29" t="n">
-        <v>1762238268</v>
+        <v>1762410501</v>
       </c>
       <c r="R29" t="n">
-        <v>530810696020</v>
+        <v>171952398500</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
@@ -4847,7 +4871,11 @@
       <c r="AE29" t="n">
         <v>5.9</v>
       </c>
-      <c r="AF29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
       <c r="AG29" t="inlineStr"/>
       <c r="AH29" t="inlineStr">
         <is>
@@ -4855,46 +4883,50 @@
         </is>
       </c>
       <c r="AI29" t="n">
-        <v>19141</v>
+        <v>19941</v>
       </c>
       <c r="AJ29" t="inlineStr">
         <is>
-          <t>263014,264517</t>
+          <t>265891</t>
         </is>
       </c>
       <c r="AK29" t="inlineStr">
         <is>
-          <t>2037,2043</t>
-        </is>
-      </c>
-      <c r="AL29" t="inlineStr"/>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="AL29" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>16868</v>
+        <v>17163</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MULAGAPAKA SALOMI</t>
+          <t>MUHAMMAD ZAYN KHAN</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9059539555</v>
+        <v>8210638795</v>
       </c>
       <c r="D30" t="n">
-        <v>8550</v>
+        <v>6750</v>
       </c>
       <c r="E30" t="n">
-        <v>8550</v>
+        <v>6750</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>04-Nov-2025 12:11:55</t>
+          <t>06-Nov-2025 18:52:13</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>06-Nov-2025 00:00:00</t>
+          <t>07-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -4909,12 +4941,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>eight thousand five hundred fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L30" t="n">
@@ -4932,13 +4964,13 @@
         <v>1234</v>
       </c>
       <c r="P30" t="n">
-        <v>11000314457730</v>
+        <v>11000314978042</v>
       </c>
       <c r="Q30" t="n">
-        <v>1762238461</v>
+        <v>1762435169</v>
       </c>
       <c r="R30" t="n">
-        <v>530810708858</v>
+        <v>531025519957</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
@@ -4997,7 +5029,7 @@
       </c>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -5007,48 +5039,42 @@
         </is>
       </c>
       <c r="AI30" t="n">
-        <v>18488</v>
+        <v>19878</v>
       </c>
       <c r="AJ30" t="inlineStr">
         <is>
-          <t>262203,263832</t>
+          <t>263393</t>
         </is>
       </c>
       <c r="AK30" t="inlineStr">
         <is>
-          <t>2037,2041</t>
+          <t>2039</t>
         </is>
       </c>
       <c r="AL30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>17264</v>
+        <v>17278</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SILUGURI CHIYAN ESHAN VARMA</t>
+          <t>PENAKADITHI SAMUEL</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>8639375454</v>
+        <v>9030736744</v>
       </c>
       <c r="D31" t="n">
-        <v>7750</v>
-      </c>
-      <c r="E31" t="n">
-        <v>7750</v>
-      </c>
+        <v>6750</v>
+      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>04-Nov-2025 14:59:32</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 00:00:00</t>
-        </is>
-      </c>
+          <t>07-Nov-2025 11:25:40</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
@@ -5061,12 +5087,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>lVl</t>
+          <t>PREKGUKG</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>seven thousand seven hundred fifty</t>
+          <t>six thousand seven hundred fifty</t>
         </is>
       </c>
       <c r="L31" t="n">
@@ -5084,13 +5110,13 @@
         <v>1234</v>
       </c>
       <c r="P31" t="n">
-        <v>11000314506510</v>
+        <v>11000315150336</v>
       </c>
       <c r="Q31" t="n">
-        <v>1762248487</v>
+        <v>1762494891</v>
       </c>
       <c r="R31" t="n">
-        <v>530811667162</v>
+        <v>531128921024</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -5109,7 +5135,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>NRNS</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
@@ -5132,24 +5158,18 @@
           <t>kotakschoolvsp@gmail.com</t>
         </is>
       </c>
-      <c r="AA31" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
       <c r="AC31" t="n">
         <v>0</v>
       </c>
       <c r="AD31" t="n">
         <v>0</v>
       </c>
-      <c r="AE31" t="n">
-        <v>5.9</v>
-      </c>
+      <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -5159,923 +5179,19 @@
         </is>
       </c>
       <c r="AI31" t="n">
-        <v>19975</v>
+        <v>19989</v>
       </c>
       <c r="AJ31" t="inlineStr">
         <is>
-          <t>263624</t>
+          <t>265141</t>
         </is>
       </c>
       <c r="AK31" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>2047</t>
         </is>
       </c>
       <c r="AL31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>17188</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>REYANA SRIJITH</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>9985925345</v>
-      </c>
-      <c r="D32" t="n">
-        <v>8250</v>
-      </c>
-      <c r="E32" t="n">
-        <v>8250</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>04-Nov-2025 23:11:27</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 00:00:00</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>lVl</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>eight thousand two hundred fifty</t>
-        </is>
-      </c>
-      <c r="L32" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N32" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O32" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P32" t="n">
-        <v>11000314605606</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>1762278029</v>
-      </c>
-      <c r="R32" t="n">
-        <v>530814184976</v>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V32" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X32" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z32" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA32" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="AF32" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
-        </is>
-      </c>
-      <c r="AG32" t="inlineStr"/>
-      <c r="AH32" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI32" t="n">
-        <v>19902</v>
-      </c>
-      <c r="AJ32" t="inlineStr">
-        <is>
-          <t>262289,263690</t>
-        </is>
-      </c>
-      <c r="AK32" t="inlineStr">
-        <is>
-          <t>2037,2040</t>
-        </is>
-      </c>
-      <c r="AL32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>16885</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>JOITA CHETTI</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>8106613759</v>
-      </c>
-      <c r="D33" t="n">
-        <v>16000</v>
-      </c>
-      <c r="E33" t="n">
-        <v>16000</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>05-Nov-2025 07:54:02</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 00:00:00</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>lVl</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">sixteen thousand </t>
-        </is>
-      </c>
-      <c r="L33" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N33" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O33" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P33" t="n">
-        <v>11000314620667</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>1762309313</v>
-      </c>
-      <c r="R33" t="n">
-        <v>530915626358</v>
-      </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V33" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="W33" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X33" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y33" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z33" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA33" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE33" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="AF33" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
-        </is>
-      </c>
-      <c r="AG33" t="inlineStr"/>
-      <c r="AH33" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI33" t="n">
-        <v>18185</v>
-      </c>
-      <c r="AJ33" t="inlineStr">
-        <is>
-          <t>262047,263508,265158</t>
-        </is>
-      </c>
-      <c r="AK33" t="inlineStr">
-        <is>
-          <t>2037,2040,2048</t>
-        </is>
-      </c>
-      <c r="AL33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>16974</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>KADAJARI ESHAN ESWAR</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>9885130099</v>
-      </c>
-      <c r="D34" t="n">
-        <v>8250</v>
-      </c>
-      <c r="E34" t="n">
-        <v>8250</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 09:44:46</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>07-Nov-2025 00:00:00</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>lVl</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>eight thousand two hundred fifty</t>
-        </is>
-      </c>
-      <c r="L34" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N34" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O34" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P34" t="n">
-        <v>11000314846264</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>1762401796</v>
-      </c>
-      <c r="R34" t="n">
-        <v>531022524983</v>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X34" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z34" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA34" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB34" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AC34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE34" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="AF34" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
-        </is>
-      </c>
-      <c r="AG34" t="inlineStr"/>
-      <c r="AH34" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI34" t="n">
-        <v>18273</v>
-      </c>
-      <c r="AJ34" t="inlineStr">
-        <is>
-          <t>262526,263740</t>
-        </is>
-      </c>
-      <c r="AK34" t="inlineStr">
-        <is>
-          <t>2037,2040</t>
-        </is>
-      </c>
-      <c r="AL34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>17229</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>GOLAGANI SOHITHA SAI SANJANA</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>9985965602</v>
-      </c>
-      <c r="D35" t="n">
-        <v>8350</v>
-      </c>
-      <c r="E35" t="n">
-        <v>8350</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 11:59:04</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>07-Nov-2025 00:00:00</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>lVl</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>eight thousand three hundred fifty</t>
-        </is>
-      </c>
-      <c r="L35" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N35" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O35" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P35" t="n">
-        <v>11000314879817</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>1762410501</v>
-      </c>
-      <c r="R35" t="n">
-        <v>171952398500</v>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T35" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V35" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X35" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z35" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA35" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB35" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AC35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE35" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="AF35" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
-        </is>
-      </c>
-      <c r="AG35" t="inlineStr"/>
-      <c r="AH35" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI35" t="n">
-        <v>19941</v>
-      </c>
-      <c r="AJ35" t="inlineStr">
-        <is>
-          <t>265891</t>
-        </is>
-      </c>
-      <c r="AK35" t="inlineStr">
-        <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="AL35" t="inlineStr">
-        <is>
-          <t>UPI INTENT</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>17163</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>MUHAMMAD ZAYN KHAN</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>8210638795</v>
-      </c>
-      <c r="D36" t="n">
-        <v>6750</v>
-      </c>
-      <c r="E36" t="n">
-        <v>6750</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>06-Nov-2025 18:52:13</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>07-Nov-2025 00:00:00</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>PREKGUKG</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>six thousand seven hundred fifty</t>
-        </is>
-      </c>
-      <c r="L36" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N36" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O36" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P36" t="n">
-        <v>11000314978042</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>1762435169</v>
-      </c>
-      <c r="R36" t="n">
-        <v>531025519957</v>
-      </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T36" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V36" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X36" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z36" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA36" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB36" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AC36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE36" t="n">
-        <v>5.9</v>
-      </c>
-      <c r="AF36" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
-        </is>
-      </c>
-      <c r="AG36" t="inlineStr"/>
-      <c r="AH36" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI36" t="n">
-        <v>19878</v>
-      </c>
-      <c r="AJ36" t="inlineStr">
-        <is>
-          <t>263393</t>
-        </is>
-      </c>
-      <c r="AK36" t="inlineStr">
-        <is>
-          <t>2039</t>
-        </is>
-      </c>
-      <c r="AL36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>17278</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>PENAKADITHI SAMUEL</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>9030736744</v>
-      </c>
-      <c r="D37" t="n">
-        <v>6750</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>07-Nov-2025 11:25:40</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>TRANSACTION IS SUCCESSFUL</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>PREKGUKG</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>six thousand seven hundred fifty</t>
-        </is>
-      </c>
-      <c r="L37" t="n">
-        <v>100000036600</v>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>SALESIAN EDUCATION SOCIETY</t>
-        </is>
-      </c>
-      <c r="N37" t="n">
-        <v>753702</v>
-      </c>
-      <c r="O37" t="n">
-        <v>1234</v>
-      </c>
-      <c r="P37" t="n">
-        <v>11000315150336</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>1762494891</v>
-      </c>
-      <c r="R37" t="n">
-        <v>531128921024</v>
-      </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>INR</t>
-        </is>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>sale</t>
-        </is>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>ICICI UPI QR</t>
-        </is>
-      </c>
-      <c r="V37" t="inlineStr">
-        <is>
-          <t>NRNS</t>
-        </is>
-      </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>SIBL0000899</t>
-        </is>
-      </c>
-      <c r="X37" t="inlineStr">
-        <is>
-          <t>MERCHANT</t>
-        </is>
-      </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>UPI</t>
-        </is>
-      </c>
-      <c r="Z37" t="inlineStr">
-        <is>
-          <t>kotakschoolvsp@gmail.com</t>
-        </is>
-      </c>
-      <c r="AA37" t="inlineStr"/>
-      <c r="AB37" t="inlineStr"/>
-      <c r="AC37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE37" t="inlineStr"/>
-      <c r="AF37" t="inlineStr">
-        <is>
-          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
-        </is>
-      </c>
-      <c r="AG37" t="inlineStr"/>
-      <c r="AH37" t="inlineStr">
-        <is>
-          <t>REGULAR</t>
-        </is>
-      </c>
-      <c r="AI37" t="n">
-        <v>19989</v>
-      </c>
-      <c r="AJ37" t="inlineStr">
-        <is>
-          <t>265141</t>
-        </is>
-      </c>
-      <c r="AK37" t="inlineStr">
-        <is>
-          <t>2047</t>
-        </is>
-      </c>
-      <c r="AL37" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>